<commit_message>
feat: Add individual card price trend tracking and display in the HTML report.
</commit_message>
<xml_diff>
--- a/MY_COLLECTION_PRICES.xlsx
+++ b/MY_COLLECTION_PRICES.xlsx
@@ -467,7 +467,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2025-12-04</t>
+          <t>2025-12-13</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -487,19 +487,19 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>2.30</t>
+          <t>2.36</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>x2 (P/L: $-0.70)</t>
+          <t>x2 (P/L: $-0.64)</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2025-12-04</t>
+          <t>2025-12-13</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -519,19 +519,19 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>0.24</t>
+          <t>0.25</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t xml:space="preserve"> (P/L: $-4.76)</t>
+          <t xml:space="preserve"> (P/L: $-4.75)</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2025-12-04</t>
+          <t>2025-12-13</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -551,7 +551,7 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>0.06</t>
+          <t>0.07</t>
         </is>
       </c>
       <c r="F4" t="inlineStr"/>
@@ -559,7 +559,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2025-12-04</t>
+          <t>2025-12-13</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -587,7 +587,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2025-12-04</t>
+          <t>2025-12-13</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -623,12 +623,12 @@
       <c r="D7" t="inlineStr"/>
       <c r="E7" t="inlineStr">
         <is>
-          <t>2.60</t>
+          <t>2.68</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Total P/L: $-5.46</t>
+          <t>Total P/L: $-5.39</t>
         </is>
       </c>
     </row>

</xml_diff>